<commit_message>
implemnt code refractor to edit translations
</commit_message>
<xml_diff>
--- a/public/downloads/translations.xlsx
+++ b/public/downloads/translations.xlsx
@@ -25,7 +25,7 @@
     <t>Locale Id</t>
   </si>
   <si>
-    <t>Text from update request</t>
+    <t>Hi Programmers</t>
   </si>
 </sst>
 </file>
@@ -440,10 +440,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1">
@@ -452,32 +452,32 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" algorithmName="SHA-512" hashValue="LP04x/HcDnfkQKXdaHBFlrYLDXzL7hayeAF9D22P1cMj6Gzw4C9I5WlQyu2e+odOJv+bgzGXQ63DJ4BFaaS23g==" saltValue="esrY2kJp4T9cTedn//TQlA==" spinCount="100000"/>
+  <sheetProtection sheet="1" formatColumns="0" formatRows="0" algorithmName="SHA-512" hashValue="PVGma0vwpgfjIKixqOV0rGn033f4LYVqrWoY6ubejA83WrTHNqWX89grkPTwKJq9IK8gqOMGXlY5KueUWfXfyg==" saltValue="Ys8ZCzKDCI28JYa83ZxEUg==" spinCount="100000"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
   <headerFooter>

</xml_diff>